<commit_message>
updated some quad tree stuff
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
   <si>
     <t>finalize binary heap</t>
   </si>
@@ -131,9 +131,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Items</t>
-  </si>
-  <si>
     <t>need to build item generator in item factory</t>
   </si>
   <si>
@@ -168,6 +165,48 @@
   </si>
   <si>
     <t>need to make world art</t>
+  </si>
+  <si>
+    <t>itemization</t>
+  </si>
+  <si>
+    <t>Itemization</t>
+  </si>
+  <si>
+    <t>implement "loot drops"</t>
+  </si>
+  <si>
+    <t>Abilities</t>
+  </si>
+  <si>
+    <t>need to implement ablities</t>
+  </si>
+  <si>
+    <t>Affects</t>
+  </si>
+  <si>
+    <t>need to implement affects</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>implement the bus process class</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>ensure that the IBusComponent class is complete</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>complete</t>
   </si>
 </sst>
 </file>
@@ -203,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -214,13 +253,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -229,10 +280,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -245,14 +293,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tasks" displayName="tasks" ref="B4:F28" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="B4:F28"/>
-  <tableColumns count="5">
-    <tableColumn id="4" name="Id" dataDxfId="0"/>
-    <tableColumn id="1" name="Assembly" dataDxfId="1"/>
-    <tableColumn id="2" name="Topic" dataDxfId="4"/>
-    <tableColumn id="3" name="Description" dataDxfId="3"/>
-    <tableColumn id="5" name="Status"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tasks" displayName="tasks" ref="B4:G35" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="B4:G35"/>
+  <tableColumns count="6">
+    <tableColumn id="4" name="Id" dataDxfId="5"/>
+    <tableColumn id="1" name="Assembly" dataDxfId="4"/>
+    <tableColumn id="2" name="Topic" dataDxfId="3"/>
+    <tableColumn id="3" name="Description" dataDxfId="2"/>
+    <tableColumn id="5" name="Status" dataDxfId="1"/>
+    <tableColumn id="6" name="Phase" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -545,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F28"/>
+  <dimension ref="B2:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,14 +607,15 @@
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="45.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
@@ -573,7 +623,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>6</v>
@@ -581,8 +631,11 @@
       <c r="F4" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -595,10 +648,14 @@
       <c r="E5" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
-        <f>B5+1</f>
+        <f t="shared" ref="B6:B33" si="0">B5+1</f>
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -610,10 +667,14 @@
       <c r="E6" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
-        <f>B6+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -625,10 +686,16 @@
       <c r="E7" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
-        <f>B7+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -640,8 +707,14 @@
       <c r="E8" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <f>B8+1</f>
         <v>5</v>
@@ -655,10 +728,12 @@
       <c r="E9" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
-        <f>B9+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -668,12 +743,14 @@
         <v>12</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
-        <f>B10+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -685,10 +762,12 @@
       <c r="E11" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
-        <f>B11+1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -700,10 +779,12 @@
       <c r="E12" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
-        <f>B12+1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -715,10 +796,12 @@
       <c r="E13" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
-        <f>B13+1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -730,10 +813,12 @@
       <c r="E14" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
-        <f>B14+1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -745,10 +830,12 @@
       <c r="E15" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
-        <f>B15+1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -760,10 +847,12 @@
       <c r="E16" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
-        <f>B16+1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -775,10 +864,12 @@
       <c r="E17" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
-        <f>B17+1</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -790,10 +881,12 @@
       <c r="E18" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
-        <f>B18+1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -805,10 +898,12 @@
       <c r="E19" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
-        <f>B19+1</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -820,10 +915,12 @@
       <c r="E20" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
-        <f>B20+1</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -835,111 +932,232 @@
       <c r="E21" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
-        <f>B21+1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
-        <f>B22+1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
-        <f>B23+1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
-        <f>B24+1</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
-        <f>B25+1</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
-        <f>B26+1</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="1">
-        <f>B27+1</f>
-        <v>24</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E28" s="3" t="s">
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="E29" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+      <c r="C34" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+      <c r="C35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
more task-list item completions
revamped StartScreen to use Glimpse
revamped timed dialog
added ButtonMenu
added DialogTimer
tweaked AStarPathfinding to path better
tweaked AI to properly reset path info, now more stable
added mouse pointer graphic
BinaryHeap can now use bracket accessors
updated task list
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="72">
   <si>
     <t>finalize binary heap</t>
   </si>
@@ -35,9 +35,6 @@
     <t>replace timed dialog window with glimpse structures</t>
   </si>
   <si>
-    <t>make main menu use glimpse</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -216,6 +213,27 @@
   </si>
   <si>
     <t>create and define a stats system</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>make main menu use glimpse - create menu manager in Vaerydian made up of a canvas background and several buttons… use the on-click to determine necessary fucntions… possibly through an event list…</t>
+  </si>
+  <si>
+    <t>GButton</t>
+  </si>
+  <si>
+    <t>update buttons to use  color modification and transparancy</t>
+  </si>
+  <si>
+    <t>StartScreen</t>
+  </si>
+  <si>
+    <t>update menu art</t>
   </si>
 </sst>
 </file>
@@ -269,7 +287,16 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -281,12 +308,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -302,15 +323,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tasks" displayName="tasks" ref="B4:G35" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="B4:G35"/>
-  <tableColumns count="6">
-    <tableColumn id="4" name="Id" dataDxfId="5"/>
-    <tableColumn id="1" name="Assembly" dataDxfId="4"/>
-    <tableColumn id="2" name="Topic" dataDxfId="3"/>
-    <tableColumn id="3" name="Description" dataDxfId="2"/>
-    <tableColumn id="5" name="Status" dataDxfId="1"/>
-    <tableColumn id="6" name="Phase" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tasks" displayName="tasks" ref="B4:H37" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="B4:H37">
+    <filterColumn colId="4">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
+  <sortState ref="B10:H37">
+    <sortCondition ref="H4:H37"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="4" name="Id" dataDxfId="0"/>
+    <tableColumn id="1" name="Assembly" dataDxfId="1"/>
+    <tableColumn id="2" name="Topic" dataDxfId="6"/>
+    <tableColumn id="3" name="Description" dataDxfId="5"/>
+    <tableColumn id="5" name="Status" dataDxfId="4"/>
+    <tableColumn id="6" name="Phase" dataDxfId="3"/>
+    <tableColumn id="7" name="Priority" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -603,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G35"/>
+  <dimension ref="B2:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,578 +646,701 @@
     <col min="5" max="5" width="45.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="1">
+        <v>55</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="4">
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
         <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G5" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="1">
-        <f t="shared" ref="B6:B35" si="0">B5+1</f>
+      <c r="H5" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G6" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="1">
-        <f t="shared" si="0"/>
+      <c r="H6" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G7" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
-        <f t="shared" si="0"/>
+      <c r="H7" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G8" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="1">
-        <f>B8+1</f>
+      <c r="H8" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="G9" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="1">
-        <f t="shared" si="0"/>
-        <v>6</v>
+      <c r="H9" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="1">
-        <f t="shared" si="0"/>
-        <v>7</v>
+      <c r="G10" s="4">
+        <v>4</v>
+      </c>
+      <c r="H10" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4">
+        <v>3</v>
+      </c>
+      <c r="H11" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="4"/>
+        <v>67</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="G12" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="1">
-        <f t="shared" si="0"/>
-        <v>9</v>
+      <c r="H12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="1">
-        <f t="shared" si="0"/>
-        <v>10</v>
+      <c r="G13" s="4">
+        <v>3</v>
+      </c>
+      <c r="H13" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>28</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="1">
-        <f t="shared" si="0"/>
+      <c r="G14" s="4">
+        <v>3</v>
+      </c>
+      <c r="H14" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4">
+        <v>3</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="1">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E16" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="1">
-        <f t="shared" si="0"/>
-        <v>13</v>
+      <c r="H16" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="4">
+        <v>12</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="1">
-        <f t="shared" si="0"/>
+      <c r="H17" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1">
-        <f t="shared" si="0"/>
-        <v>15</v>
+      <c r="H18" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
+        <v>14</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="1">
-        <f t="shared" si="0"/>
-        <v>16</v>
+      <c r="H19" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="4">
+        <v>15</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="1">
-        <f t="shared" si="0"/>
-        <v>17</v>
+      <c r="H20" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="4">
+        <v>16</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="1">
-        <f t="shared" si="0"/>
-        <v>18</v>
+      <c r="H21" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
+        <v>17</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="1">
-        <f t="shared" si="0"/>
-        <v>19</v>
+      <c r="H22" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
+        <v>18</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="1">
-        <f t="shared" si="0"/>
-        <v>20</v>
+      <c r="H23" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
+        <v>19</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="1">
-        <f t="shared" si="0"/>
-        <v>21</v>
+      <c r="H24" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <v>20</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="1">
-        <f t="shared" si="0"/>
-        <v>22</v>
+      <c r="H25" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
+        <v>26</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="1">
-        <f t="shared" si="0"/>
-        <v>23</v>
+      <c r="H26" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
+        <v>27</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="1">
-        <f t="shared" si="0"/>
-        <v>24</v>
+      <c r="H27" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="4">
+        <v>7</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="1">
-        <f t="shared" si="0"/>
-        <v>25</v>
+      <c r="H28" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="4">
+        <v>21</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="1">
-        <f t="shared" si="0"/>
-        <v>26</v>
+      <c r="H29" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="4">
+        <v>22</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="1">
-        <f t="shared" si="0"/>
-        <v>27</v>
+      <c r="H30" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="4">
+        <v>23</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="1">
-        <f t="shared" si="0"/>
-        <v>28</v>
+      <c r="H31" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="4">
+        <v>24</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="1">
-        <f t="shared" si="0"/>
-        <v>29</v>
+      <c r="H32" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="4">
+        <v>25</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B34" s="1">
-        <f t="shared" si="0"/>
+      <c r="H33" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B34" s="4">
         <v>30</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="1">
-        <f t="shared" si="0"/>
+      <c r="H34" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="4">
         <v>31</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
+      <c r="H35" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="4">
+        <v>32</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G36" s="4">
+        <v>2</v>
+      </c>
+      <c r="H36" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="4">
+        <v>32</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1213,37 +1365,37 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
various tweaks, fixed mapdebug inclusion issue
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="102">
   <si>
     <t>finalize binary heap</t>
   </si>
@@ -284,9 +284,6 @@
     <t>handle requesting retrieves</t>
   </si>
   <si>
-    <t>in-work</t>
-  </si>
-  <si>
     <t>Bus Registration</t>
   </si>
   <si>
@@ -297,6 +294,36 @@
   </si>
   <si>
     <t>make sure that the mouse reticle is drawn over everything… meaning its drawn last…</t>
+  </si>
+  <si>
+    <t>postponed</t>
+  </si>
+  <si>
+    <t>generators for other terrain types</t>
+  </si>
+  <si>
+    <t>Art</t>
+  </si>
+  <si>
+    <t>terrain</t>
+  </si>
+  <si>
+    <t>come up with terrain art</t>
+  </si>
+  <si>
+    <t>come up with color variations for each terrain</t>
+  </si>
+  <si>
+    <t>MapSystem</t>
+  </si>
+  <si>
+    <t>move world art into pre-load</t>
+  </si>
+  <si>
+    <t>update buttons to use text and change the text color on mouse inputs etc.</t>
+  </si>
+  <si>
+    <t>correct width calculation bug in buttons</t>
   </si>
 </sst>
 </file>
@@ -386,8 +413,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tasks" displayName="tasks" ref="B4:H49" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="B4:H49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tasks" displayName="tasks" ref="B4:H55" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="B4:H55"/>
   <sortState ref="B5:H48">
     <sortCondition ref="B4:B48"/>
   </sortState>
@@ -691,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H49"/>
+  <dimension ref="B2:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,7 +977,9 @@
       <c r="E14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="G14" s="4">
         <v>4</v>
       </c>
@@ -971,7 +1000,9 @@
       <c r="E15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="4"/>
+      <c r="F15" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="G15" s="4">
         <v>4</v>
       </c>
@@ -1296,7 +1327,9 @@
       <c r="E32" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F32" s="4"/>
+      <c r="F32" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="G32" s="4">
         <v>4</v>
       </c>
@@ -1317,7 +1350,9 @@
       <c r="E33" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F33" s="4"/>
+      <c r="F33" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="G33" s="4">
         <v>4</v>
       </c>
@@ -1579,7 +1614,9 @@
       <c r="E45" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F45" s="4"/>
+      <c r="F45" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="G45" s="4">
         <v>4</v>
       </c>
@@ -1641,13 +1678,13 @@
         <v>15</v>
       </c>
       <c r="D48" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E48" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="F48" s="4" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="G48" s="4">
         <v>4</v>
@@ -1664,16 +1701,120 @@
         <v>7</v>
       </c>
       <c r="D49" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
       <c r="H49" s="4">
         <v>3</v>
       </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="4">
+        <v>45</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="4">
+        <v>46</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="4">
+        <v>47</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="4">
+        <v>48</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B54" s="4">
+        <v>49</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="4">
+        <v>50</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed bag namespace issues
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="110">
   <si>
     <t>finalize binary heap</t>
   </si>
@@ -324,6 +324,30 @@
   </si>
   <si>
     <t>correct width calculation bug in buttons</t>
+  </si>
+  <si>
+    <t>character inventory ui</t>
+  </si>
+  <si>
+    <t>character stat ui</t>
+  </si>
+  <si>
+    <t>NPC Factory</t>
+  </si>
+  <si>
+    <t>need to create more types of mobs</t>
+  </si>
+  <si>
+    <t>Factories</t>
+  </si>
+  <si>
+    <t>need to define method for factories to assemble mob templates</t>
+  </si>
+  <si>
+    <t>Systems</t>
+  </si>
+  <si>
+    <t>Need to define a Trigger system and Trigger Component</t>
   </si>
 </sst>
 </file>
@@ -413,8 +437,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tasks" displayName="tasks" ref="B4:H55" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="B4:H55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tasks" displayName="tasks" ref="B4:H60" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="B4:H60">
+    <filterColumn colId="4">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="B5:H48">
     <sortCondition ref="B4:B48"/>
   </sortState>
@@ -718,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H55"/>
+  <dimension ref="B2:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,7 +791,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>1</v>
       </c>
@@ -786,7 +814,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>2</v>
       </c>
@@ -809,7 +837,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <v>3</v>
       </c>
@@ -832,7 +860,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>4</v>
       </c>
@@ -855,7 +883,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>5</v>
       </c>
@@ -878,7 +906,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>6</v>
       </c>
@@ -920,7 +948,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>8</v>
       </c>
@@ -957,14 +985,12 @@
         <v>13</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="4">
-        <v>5</v>
-      </c>
+      <c r="G13" s="4"/>
       <c r="H13" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>10</v>
       </c>
@@ -987,7 +1013,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>11</v>
       </c>
@@ -1102,7 +1128,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -1121,7 +1147,7 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -1314,7 +1340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" s="4">
         <v>28</v>
       </c>
@@ -1337,7 +1363,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4">
         <v>29</v>
       </c>
@@ -1379,7 +1405,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" s="4">
         <v>31</v>
       </c>
@@ -1402,7 +1428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="4">
         <v>32</v>
       </c>
@@ -1444,7 +1470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" s="4">
         <v>33</v>
       </c>
@@ -1467,7 +1493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B39" s="4">
         <v>34</v>
       </c>
@@ -1490,7 +1516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B40" s="4">
         <v>35</v>
       </c>
@@ -1513,7 +1539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41" s="4">
         <v>36</v>
       </c>
@@ -1555,7 +1581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B43" s="4">
         <v>38</v>
       </c>
@@ -1578,7 +1604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B44" s="4">
         <v>39</v>
       </c>
@@ -1601,7 +1627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B45" s="4">
         <v>40</v>
       </c>
@@ -1624,7 +1650,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B46" s="4">
         <v>41</v>
       </c>
@@ -1647,7 +1673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47" s="4">
         <v>42</v>
       </c>
@@ -1670,7 +1696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B48" s="4">
         <v>43</v>
       </c>
@@ -1727,7 +1753,9 @@
       </c>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
+      <c r="H50" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="4">
@@ -1744,7 +1772,9 @@
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
+      <c r="H51" s="4">
+        <v>4</v>
+      </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="4">
@@ -1761,7 +1791,9 @@
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
+      <c r="H52" s="4">
+        <v>4</v>
+      </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" s="4">
@@ -1778,9 +1810,11 @@
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
-    </row>
-    <row r="54" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H53" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B54" s="4">
         <v>49</v>
       </c>
@@ -1814,7 +1848,102 @@
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
+      <c r="H55" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="4">
+        <v>51</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="4">
+        <v>52</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="4">
+        <v>53</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B59" s="4">
+        <v>54</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B60" s="4">
+        <v>55</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>